<commit_message>
Fixing Validation, excel, login and maintenance.
</commit_message>
<xml_diff>
--- a/debtchecking/TemplateFile/template.xlsx
+++ b/debtchecking/TemplateFile/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JOGJA\SKBF\Source Code\edisweb\debtchecking\TemplateFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E4AB3C-89F8-4938-8035-5FEC51D185DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6722B8-7A0F-4603-B555-47B479A5E0B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{502649AF-9EC9-476A-A048-41000DCD0846}"/>
   </bookViews>
@@ -12350,8 +12350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1005E8CB-A649-4733-AF1C-9C08982D3EF3}">
   <dimension ref="A1:AD102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:R1"/>
+    <sheetView tabSelected="1" topLeftCell="S102" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="U107" sqref="U107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13344,7 +13344,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="17">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="12">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Peringatan" error="Jenis Customer Tidak Valid" xr:uid="{6170CF18-095C-46A9-AAA8-B91299D7722A}">
           <x14:formula1>
             <xm:f>Parameter!$T$4:$T$5</xm:f>
@@ -13387,24 +13387,6 @@
           </x14:formula1>
           <xm:sqref>L3:L102</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C642411F-FD48-4B4A-AFB3-FC616FD91D87}">
-          <x14:formula1>
-            <xm:f>Parameter!$Y$4:$Y$301</xm:f>
-          </x14:formula1>
-          <xm:sqref>S3:S102</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CDE81096-2A78-40B4-9840-0D4B135DC7F3}">
-          <x14:formula1>
-            <xm:f>Parameter!$AD$4:$AD$695</xm:f>
-          </x14:formula1>
-          <xm:sqref>T3:T102</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4DD393E4-7BD2-4149-96CE-162EC2A51912}">
-          <x14:formula1>
-            <xm:f>Parameter!$AH$4:$AH$52</xm:f>
-          </x14:formula1>
-          <xm:sqref>U3:U102</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{58576EA0-D291-4D86-B346-B9355202BF99}">
           <x14:formula1>
             <xm:f>Parameter!$AT$4:$AT$16</xm:f>
@@ -13422,18 +13404,6 @@
             <xm:f>Parameter!$L$18:$L$19</xm:f>
           </x14:formula1>
           <xm:sqref>H3:H102</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3B8CD43B-115F-47A7-8D41-496804923E48}">
-          <x14:formula1>
-            <xm:f>Parameter!$AL$4:$AL$326</xm:f>
-          </x14:formula1>
-          <xm:sqref>V3:V102</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A33C7813-5558-4ABE-857F-69776C3B049A}">
-          <x14:formula1>
-            <xm:f>Parameter!$AP$4:$AP$1716</xm:f>
-          </x14:formula1>
-          <xm:sqref>W3:W102</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Peringatan" error="Tahun Tidak Valid" xr:uid="{04D2F5C2-1B04-4A3F-92D1-E4CFD442E83E}">
           <x14:formula1>

</xml_diff>